<commit_message>
cohort for pos controls added
</commit_message>
<xml_diff>
--- a/source_data/Metagenome.environmental_20190308_2.xlsx
+++ b/source_data/Metagenome.environmental_20190308_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8060" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
   </bookViews>
   <sheets>
     <sheet name="Metagenome.environmental.1.0" sheetId="1" r:id="rId1"/>
@@ -4164,8 +4164,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4242,7 +4244,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4260,6 +4262,7 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4277,6 +4280,7 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4578,8 +4582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE925"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="C153" sqref="C153"/>
+    <sheetView tabSelected="1" topLeftCell="R914" workbookViewId="0">
+      <selection activeCell="Y928" sqref="Y928"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -63750,7 +63754,7 @@
         <v>944</v>
       </c>
       <c r="V881" t="s">
-        <v>944</v>
+        <v>958</v>
       </c>
       <c r="W881" t="s">
         <v>944</v>
@@ -63818,7 +63822,7 @@
         <v>944</v>
       </c>
       <c r="V882" t="s">
-        <v>944</v>
+        <v>958</v>
       </c>
       <c r="W882" t="s">
         <v>944</v>
@@ -63886,7 +63890,7 @@
         <v>944</v>
       </c>
       <c r="V883" t="s">
-        <v>944</v>
+        <v>958</v>
       </c>
       <c r="W883" t="s">
         <v>944</v>
@@ -63954,7 +63958,7 @@
         <v>944</v>
       </c>
       <c r="V884" t="s">
-        <v>944</v>
+        <v>958</v>
       </c>
       <c r="W884" t="s">
         <v>944</v>
@@ -64022,7 +64026,7 @@
         <v>944</v>
       </c>
       <c r="V885" t="s">
-        <v>944</v>
+        <v>958</v>
       </c>
       <c r="W885" t="s">
         <v>944</v>
@@ -64090,7 +64094,7 @@
         <v>944</v>
       </c>
       <c r="V886" t="s">
-        <v>944</v>
+        <v>958</v>
       </c>
       <c r="W886" t="s">
         <v>944</v>
@@ -64158,7 +64162,7 @@
         <v>944</v>
       </c>
       <c r="V887" t="s">
-        <v>944</v>
+        <v>958</v>
       </c>
       <c r="W887" t="s">
         <v>944</v>
@@ -64226,7 +64230,7 @@
         <v>944</v>
       </c>
       <c r="V888" t="s">
-        <v>944</v>
+        <v>958</v>
       </c>
       <c r="W888" t="s">
         <v>944</v>
@@ -64294,7 +64298,7 @@
         <v>944</v>
       </c>
       <c r="V889" t="s">
-        <v>944</v>
+        <v>958</v>
       </c>
       <c r="W889" t="s">
         <v>944</v>
@@ -64362,7 +64366,7 @@
         <v>944</v>
       </c>
       <c r="V890" t="s">
-        <v>944</v>
+        <v>959</v>
       </c>
       <c r="W890" t="s">
         <v>944</v>
@@ -64430,7 +64434,7 @@
         <v>944</v>
       </c>
       <c r="V891" t="s">
-        <v>944</v>
+        <v>960</v>
       </c>
       <c r="W891" t="s">
         <v>944</v>
@@ -64498,7 +64502,7 @@
         <v>944</v>
       </c>
       <c r="V892" t="s">
-        <v>944</v>
+        <v>960</v>
       </c>
       <c r="W892" t="s">
         <v>944</v>
@@ -64566,7 +64570,7 @@
         <v>944</v>
       </c>
       <c r="V893" t="s">
-        <v>944</v>
+        <v>959</v>
       </c>
       <c r="W893" t="s">
         <v>944</v>
@@ -64634,7 +64638,7 @@
         <v>944</v>
       </c>
       <c r="V894" t="s">
-        <v>944</v>
+        <v>960</v>
       </c>
       <c r="W894" t="s">
         <v>944</v>
@@ -64702,7 +64706,7 @@
         <v>944</v>
       </c>
       <c r="V895" t="s">
-        <v>944</v>
+        <v>959</v>
       </c>
       <c r="W895" t="s">
         <v>944</v>
@@ -64770,7 +64774,7 @@
         <v>944</v>
       </c>
       <c r="V896" t="s">
-        <v>944</v>
+        <v>959</v>
       </c>
       <c r="W896" t="s">
         <v>944</v>
@@ -64838,7 +64842,7 @@
         <v>944</v>
       </c>
       <c r="V897" t="s">
-        <v>944</v>
+        <v>960</v>
       </c>
       <c r="W897" t="s">
         <v>944</v>
@@ -64906,7 +64910,7 @@
         <v>944</v>
       </c>
       <c r="V898" t="s">
-        <v>944</v>
+        <v>960</v>
       </c>
       <c r="W898" t="s">
         <v>944</v>
@@ -64974,7 +64978,7 @@
         <v>944</v>
       </c>
       <c r="V899" t="s">
-        <v>944</v>
+        <v>959</v>
       </c>
       <c r="W899" t="s">
         <v>944</v>
@@ -65042,7 +65046,7 @@
         <v>944</v>
       </c>
       <c r="V900" t="s">
-        <v>944</v>
+        <v>960</v>
       </c>
       <c r="W900" t="s">
         <v>944</v>
@@ -65110,7 +65114,7 @@
         <v>944</v>
       </c>
       <c r="V901" t="s">
-        <v>944</v>
+        <v>959</v>
       </c>
       <c r="W901" t="s">
         <v>944</v>
@@ -65178,7 +65182,7 @@
         <v>944</v>
       </c>
       <c r="V902" t="s">
-        <v>944</v>
+        <v>960</v>
       </c>
       <c r="W902" t="s">
         <v>944</v>
@@ -65246,7 +65250,7 @@
         <v>944</v>
       </c>
       <c r="V903" t="s">
-        <v>944</v>
+        <v>959</v>
       </c>
       <c r="W903" t="s">
         <v>944</v>
@@ -65314,7 +65318,7 @@
         <v>944</v>
       </c>
       <c r="V904" t="s">
-        <v>944</v>
+        <v>960</v>
       </c>
       <c r="W904" t="s">
         <v>944</v>
@@ -65382,7 +65386,7 @@
         <v>944</v>
       </c>
       <c r="V905" t="s">
-        <v>944</v>
+        <v>959</v>
       </c>
       <c r="W905" t="s">
         <v>944</v>
@@ -65450,7 +65454,7 @@
         <v>944</v>
       </c>
       <c r="V906" t="s">
-        <v>944</v>
+        <v>961</v>
       </c>
       <c r="W906" t="s">
         <v>944</v>
@@ -65518,7 +65522,7 @@
         <v>944</v>
       </c>
       <c r="V907" t="s">
-        <v>944</v>
+        <v>961</v>
       </c>
       <c r="W907" t="s">
         <v>944</v>
@@ -65586,7 +65590,7 @@
         <v>944</v>
       </c>
       <c r="V908" t="s">
-        <v>944</v>
+        <v>961</v>
       </c>
       <c r="W908" t="s">
         <v>944</v>
@@ -65654,7 +65658,7 @@
         <v>944</v>
       </c>
       <c r="V909" t="s">
-        <v>944</v>
+        <v>961</v>
       </c>
       <c r="W909" t="s">
         <v>944</v>
@@ -65722,7 +65726,7 @@
         <v>944</v>
       </c>
       <c r="V910" t="s">
-        <v>944</v>
+        <v>961</v>
       </c>
       <c r="W910" t="s">
         <v>944</v>
@@ -65790,7 +65794,7 @@
         <v>944</v>
       </c>
       <c r="V911" t="s">
-        <v>944</v>
+        <v>961</v>
       </c>
       <c r="W911" t="s">
         <v>944</v>
@@ -65858,7 +65862,7 @@
         <v>944</v>
       </c>
       <c r="V912" t="s">
-        <v>944</v>
+        <v>961</v>
       </c>
       <c r="W912" t="s">
         <v>944</v>
@@ -65926,7 +65930,7 @@
         <v>944</v>
       </c>
       <c r="V913" t="s">
-        <v>944</v>
+        <v>961</v>
       </c>
       <c r="W913" t="s">
         <v>944</v>
@@ -65994,7 +65998,7 @@
         <v>944</v>
       </c>
       <c r="V914" t="s">
-        <v>944</v>
+        <v>961</v>
       </c>
       <c r="W914" t="s">
         <v>944</v>
@@ -66062,7 +66066,7 @@
         <v>944</v>
       </c>
       <c r="V915" t="s">
-        <v>944</v>
+        <v>961</v>
       </c>
       <c r="W915" t="s">
         <v>944</v>
@@ -66130,7 +66134,7 @@
         <v>944</v>
       </c>
       <c r="V916" t="s">
-        <v>944</v>
+        <v>961</v>
       </c>
       <c r="W916" t="s">
         <v>944</v>
@@ -66198,7 +66202,7 @@
         <v>944</v>
       </c>
       <c r="V917" t="s">
-        <v>944</v>
+        <v>961</v>
       </c>
       <c r="W917" t="s">
         <v>944</v>
@@ -66266,7 +66270,7 @@
         <v>944</v>
       </c>
       <c r="V918" t="s">
-        <v>944</v>
+        <v>961</v>
       </c>
       <c r="W918" t="s">
         <v>944</v>
@@ -66334,7 +66338,7 @@
         <v>944</v>
       </c>
       <c r="V919" t="s">
-        <v>944</v>
+        <v>961</v>
       </c>
       <c r="W919" t="s">
         <v>944</v>
@@ -66402,7 +66406,7 @@
         <v>944</v>
       </c>
       <c r="V920" t="s">
-        <v>944</v>
+        <v>961</v>
       </c>
       <c r="W920" t="s">
         <v>944</v>
@@ -66470,7 +66474,7 @@
         <v>944</v>
       </c>
       <c r="V921" t="s">
-        <v>944</v>
+        <v>961</v>
       </c>
       <c r="W921" t="s">
         <v>944</v>
@@ -66538,7 +66542,7 @@
         <v>944</v>
       </c>
       <c r="V922" t="s">
-        <v>944</v>
+        <v>961</v>
       </c>
       <c r="W922" t="s">
         <v>944</v>
@@ -66606,7 +66610,7 @@
         <v>944</v>
       </c>
       <c r="V923" t="s">
-        <v>944</v>
+        <v>961</v>
       </c>
       <c r="W923" t="s">
         <v>944</v>
@@ -66674,7 +66678,7 @@
         <v>944</v>
       </c>
       <c r="V924" t="s">
-        <v>944</v>
+        <v>961</v>
       </c>
       <c r="W924" t="s">
         <v>944</v>

</xml_diff>

<commit_message>
edited cohort info for pos controls
</commit_message>
<xml_diff>
--- a/source_data/Metagenome.environmental_20190308_2.xlsx
+++ b/source_data/Metagenome.environmental_20190308_2.xlsx
@@ -295,7 +295,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16645" uniqueCount="1129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16645" uniqueCount="1131">
   <si>
     <r>
       <rPr>
@@ -3972,6 +3972,12 @@
   </si>
   <si>
     <t>Sow</t>
+  </si>
+  <si>
+    <t>PosControl_ColiGuard</t>
+  </si>
+  <si>
+    <t>PosControl_Protexin</t>
   </si>
 </sst>
 </file>
@@ -4164,8 +4170,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4244,7 +4268,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4263,6 +4287,15 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4281,6 +4314,15 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4582,8 +4624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE925"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R914" workbookViewId="0">
-      <selection activeCell="Y928" sqref="Y928"/>
+    <sheetView tabSelected="1" topLeftCell="R877" workbookViewId="0">
+      <selection activeCell="V896" sqref="V896"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4602,6 +4644,7 @@
     <col min="15" max="15" width="11.6640625" style="1" customWidth="1"/>
     <col min="16" max="16" width="20.6640625" style="1" customWidth="1"/>
     <col min="17" max="17" width="13.6640625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="29.5" customWidth="1"/>
     <col min="26" max="26" width="24.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -64366,7 +64409,7 @@
         <v>944</v>
       </c>
       <c r="V890" t="s">
-        <v>959</v>
+        <v>1129</v>
       </c>
       <c r="W890" t="s">
         <v>944</v>
@@ -64434,7 +64477,7 @@
         <v>944</v>
       </c>
       <c r="V891" t="s">
-        <v>960</v>
+        <v>1130</v>
       </c>
       <c r="W891" t="s">
         <v>944</v>
@@ -64502,7 +64545,7 @@
         <v>944</v>
       </c>
       <c r="V892" t="s">
-        <v>960</v>
+        <v>1130</v>
       </c>
       <c r="W892" t="s">
         <v>944</v>
@@ -64570,7 +64613,7 @@
         <v>944</v>
       </c>
       <c r="V893" t="s">
-        <v>959</v>
+        <v>1129</v>
       </c>
       <c r="W893" t="s">
         <v>944</v>
@@ -64638,7 +64681,7 @@
         <v>944</v>
       </c>
       <c r="V894" t="s">
-        <v>960</v>
+        <v>1130</v>
       </c>
       <c r="W894" t="s">
         <v>944</v>
@@ -64706,7 +64749,7 @@
         <v>944</v>
       </c>
       <c r="V895" t="s">
-        <v>959</v>
+        <v>1129</v>
       </c>
       <c r="W895" t="s">
         <v>944</v>
@@ -64774,7 +64817,7 @@
         <v>944</v>
       </c>
       <c r="V896" t="s">
-        <v>959</v>
+        <v>1129</v>
       </c>
       <c r="W896" t="s">
         <v>944</v>
@@ -64842,7 +64885,7 @@
         <v>944</v>
       </c>
       <c r="V897" t="s">
-        <v>960</v>
+        <v>1130</v>
       </c>
       <c r="W897" t="s">
         <v>944</v>
@@ -64910,7 +64953,7 @@
         <v>944</v>
       </c>
       <c r="V898" t="s">
-        <v>960</v>
+        <v>1130</v>
       </c>
       <c r="W898" t="s">
         <v>944</v>
@@ -64978,7 +65021,7 @@
         <v>944</v>
       </c>
       <c r="V899" t="s">
-        <v>959</v>
+        <v>1129</v>
       </c>
       <c r="W899" t="s">
         <v>944</v>
@@ -65046,7 +65089,7 @@
         <v>944</v>
       </c>
       <c r="V900" t="s">
-        <v>960</v>
+        <v>1130</v>
       </c>
       <c r="W900" t="s">
         <v>944</v>
@@ -65114,7 +65157,7 @@
         <v>944</v>
       </c>
       <c r="V901" t="s">
-        <v>959</v>
+        <v>1129</v>
       </c>
       <c r="W901" t="s">
         <v>944</v>
@@ -65182,7 +65225,7 @@
         <v>944</v>
       </c>
       <c r="V902" t="s">
-        <v>960</v>
+        <v>1130</v>
       </c>
       <c r="W902" t="s">
         <v>944</v>
@@ -65250,7 +65293,7 @@
         <v>944</v>
       </c>
       <c r="V903" t="s">
-        <v>959</v>
+        <v>1129</v>
       </c>
       <c r="W903" t="s">
         <v>944</v>
@@ -65318,7 +65361,7 @@
         <v>944</v>
       </c>
       <c r="V904" t="s">
-        <v>960</v>
+        <v>1130</v>
       </c>
       <c r="W904" t="s">
         <v>944</v>
@@ -65386,7 +65429,7 @@
         <v>944</v>
       </c>
       <c r="V905" t="s">
-        <v>959</v>
+        <v>1129</v>
       </c>
       <c r="W905" t="s">
         <v>944</v>

</xml_diff>